<commit_message>
add comments and documents
</commit_message>
<xml_diff>
--- a/datasets-used.xlsx
+++ b/datasets-used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang\Desktop\CS-GY 6513 Big Data\project1\bigdataProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E29625-A385-4908-908D-1AA50E977EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF4A8F3-DBE0-4E60-B099-C3618BE8EC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Dataset Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,6 +145,22 @@
   </si>
   <si>
     <t>country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>World COVID-19 Events Timeline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://dataverse.harvard.edu/dataset.xhtml?persistentId=doi:10.7910/DVN/OAM2JK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated to May 3, 2020. Policies and regulations released by the Chinese government, global organizations, western countries, and so on. It is categorized as Chinese News Timeline and Global News Timeline. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicine, Health and Life Sciences; Law </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -214,12 +230,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -501,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -617,13 +634,46 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43893</v>
+      </c>
+      <c r="H4" s="3">
+        <v>43955</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{5F108D9B-3C30-40A8-AFD1-CF915ADBFF1B}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{24E57778-B57B-42B4-8FC8-8959788E60F5}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{333C5646-B299-43C2-9AC6-B1DB438073FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>